<commit_message>
MCM pattern new questions
</commit_message>
<xml_diff>
--- a/450dsa/FINAL450_my.xlsx
+++ b/450dsa/FINAL450_my.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data-structures\450dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F59F09B-B871-45CF-9E68-3A7384A3C35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A484CEF-AA4B-4AAF-9F9F-261B099B26B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2138,8 +2138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
-      <selection activeCell="B459" sqref="B459"/>
+    <sheetView tabSelected="1" topLeftCell="A472" workbookViewId="0">
+      <selection activeCell="B481" sqref="B481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6985,47 +6985,47 @@
         <v>4</v>
       </c>
     </row>
-    <row r="459" spans="1:3" ht="21">
-      <c r="A459" s="5" t="s">
+    <row r="459" spans="1:3" s="50" customFormat="1" ht="21">
+      <c r="A459" s="49" t="s">
         <v>393</v>
       </c>
-      <c r="B459" s="6" t="s">
+      <c r="B459" s="27" t="s">
         <v>442</v>
       </c>
-      <c r="C459" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="460" spans="1:3" ht="21">
-      <c r="A460" s="5" t="s">
+      <c r="C459" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" s="50" customFormat="1" ht="21">
+      <c r="A460" s="49" t="s">
         <v>393</v>
       </c>
-      <c r="B460" s="6" t="s">
+      <c r="B460" s="27" t="s">
         <v>443</v>
       </c>
-      <c r="C460" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="461" spans="1:3" ht="21">
-      <c r="A461" s="5" t="s">
+      <c r="C460" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" s="50" customFormat="1" ht="21">
+      <c r="A461" s="49" t="s">
         <v>393</v>
       </c>
-      <c r="B461" s="6" t="s">
+      <c r="B461" s="27" t="s">
         <v>444</v>
       </c>
-      <c r="C461" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="462" spans="1:3" ht="21">
-      <c r="A462" s="5" t="s">
+      <c r="C461" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" s="48" customFormat="1" ht="21">
+      <c r="A462" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="B462" s="6" t="s">
+      <c r="B462" s="21" t="s">
         <v>445</v>
       </c>
-      <c r="C462" s="4" t="s">
+      <c r="C462" s="22" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7040,69 +7040,69 @@
         <v>4</v>
       </c>
     </row>
-    <row r="464" spans="1:3" ht="21">
-      <c r="A464" s="5" t="s">
+    <row r="464" spans="1:3" s="48" customFormat="1" ht="21">
+      <c r="A464" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="B464" s="6" t="s">
+      <c r="B464" s="21" t="s">
         <v>447</v>
       </c>
-      <c r="C464" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="465" spans="1:3" ht="21">
-      <c r="A465" s="5" t="s">
+      <c r="C464" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" s="48" customFormat="1" ht="21">
+      <c r="A465" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="B465" s="6" t="s">
+      <c r="B465" s="21" t="s">
         <v>448</v>
       </c>
-      <c r="C465" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="466" spans="1:3" ht="21">
-      <c r="A466" s="5" t="s">
+      <c r="C465" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" s="48" customFormat="1" ht="21">
+      <c r="A466" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="B466" s="6" t="s">
+      <c r="B466" s="21" t="s">
         <v>449</v>
       </c>
-      <c r="C466" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="467" spans="1:3" ht="21">
-      <c r="A467" s="5" t="s">
+      <c r="C466" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" s="48" customFormat="1" ht="21">
+      <c r="A467" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="B467" s="6" t="s">
+      <c r="B467" s="21" t="s">
         <v>450</v>
       </c>
-      <c r="C467" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="468" spans="1:3" ht="21">
-      <c r="A468" s="5" t="s">
+      <c r="C467" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" s="47" customFormat="1" ht="21">
+      <c r="A468" s="36" t="s">
         <v>393</v>
       </c>
-      <c r="B468" s="6" t="s">
+      <c r="B468" s="24" t="s">
         <v>451</v>
       </c>
-      <c r="C468" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="469" spans="1:3" ht="21">
-      <c r="A469" s="5" t="s">
+      <c r="C468" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" s="47" customFormat="1" ht="21">
+      <c r="A469" s="36" t="s">
         <v>393</v>
       </c>
-      <c r="B469" s="6" t="s">
+      <c r="B469" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="C469" s="4" t="s">
+      <c r="C469" s="25" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7115,14 +7115,14 @@
       <c r="B471" s="7"/>
       <c r="C471" s="4"/>
     </row>
-    <row r="472" spans="1:3" ht="21">
-      <c r="A472" s="5" t="s">
+    <row r="472" spans="1:3" s="47" customFormat="1" ht="21">
+      <c r="A472" s="36" t="s">
         <v>453</v>
       </c>
-      <c r="B472" s="6" t="s">
+      <c r="B472" s="24" t="s">
         <v>454</v>
       </c>
-      <c r="C472" s="4" t="s">
+      <c r="C472" s="25" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7137,47 +7137,47 @@
         <v>4</v>
       </c>
     </row>
-    <row r="474" spans="1:3" ht="21">
-      <c r="A474" s="5" t="s">
+    <row r="474" spans="1:3" s="47" customFormat="1" ht="21">
+      <c r="A474" s="36" t="s">
         <v>453</v>
       </c>
-      <c r="B474" s="6" t="s">
+      <c r="B474" s="24" t="s">
         <v>456</v>
       </c>
-      <c r="C474" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="475" spans="1:3" ht="21">
-      <c r="A475" s="5" t="s">
+      <c r="C474" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="475" spans="1:3" s="48" customFormat="1" ht="21">
+      <c r="A475" s="20" t="s">
         <v>453</v>
       </c>
-      <c r="B475" s="6" t="s">
+      <c r="B475" s="21" t="s">
         <v>457</v>
       </c>
-      <c r="C475" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="476" spans="1:3" ht="21">
-      <c r="A476" s="5" t="s">
+      <c r="C475" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" s="47" customFormat="1" ht="21">
+      <c r="A476" s="36" t="s">
         <v>453</v>
       </c>
-      <c r="B476" s="6" t="s">
+      <c r="B476" s="24" t="s">
         <v>458</v>
       </c>
-      <c r="C476" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="477" spans="1:3" ht="21">
-      <c r="A477" s="5" t="s">
+      <c r="C476" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" s="47" customFormat="1" ht="21">
+      <c r="A477" s="36" t="s">
         <v>453</v>
       </c>
-      <c r="B477" s="6" t="s">
+      <c r="B477" s="24" t="s">
         <v>459</v>
       </c>
-      <c r="C477" s="4" t="s">
+      <c r="C477" s="25" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started heaps from 450
</commit_message>
<xml_diff>
--- a/450dsa/FINAL450_my.xlsx
+++ b/450dsa/FINAL450_my.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data-structures\450dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A484CEF-AA4B-4AAF-9F9F-261B099B26B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A2E881-4B53-4F0C-B227-1C2017B6BA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1676,7 +1676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1821,6 +1821,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2138,8 +2141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A472" workbookViewId="0">
-      <selection activeCell="B481" sqref="B481"/>
+    <sheetView tabSelected="1" topLeftCell="A343" workbookViewId="0">
+      <selection activeCell="B348" sqref="B348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5696,36 +5699,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="338" spans="1:3" ht="21">
-      <c r="A338" s="8" t="s">
+    <row r="338" spans="1:3" s="50" customFormat="1" ht="21">
+      <c r="A338" s="26" t="s">
         <v>324</v>
       </c>
-      <c r="B338" s="6" t="s">
+      <c r="B338" s="27" t="s">
         <v>327</v>
       </c>
-      <c r="C338" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="339" spans="1:3" ht="21">
-      <c r="A339" s="8" t="s">
+      <c r="C338" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" s="47" customFormat="1" ht="21">
+      <c r="A339" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="B339" s="6" t="s">
+      <c r="B339" s="24" t="s">
         <v>328</v>
       </c>
-      <c r="C339" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="340" spans="1:3" ht="21">
-      <c r="A340" s="8" t="s">
+      <c r="C339" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" s="47" customFormat="1" ht="21">
+      <c r="A340" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="B340" s="6" t="s">
+      <c r="B340" s="24" t="s">
         <v>329</v>
       </c>
-      <c r="C340" s="4" t="s">
+      <c r="C340" s="25" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5740,14 +5743,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="342" spans="1:3" ht="21">
-      <c r="A342" s="8" t="s">
+    <row r="342" spans="1:3" s="47" customFormat="1" ht="21">
+      <c r="A342" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="B342" s="6" t="s">
+      <c r="B342" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="C342" s="4" t="s">
+      <c r="C342" s="25" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5762,47 +5765,47 @@
         <v>4</v>
       </c>
     </row>
-    <row r="344" spans="1:3" ht="21">
-      <c r="A344" s="8" t="s">
+    <row r="344" spans="1:3" s="47" customFormat="1" ht="21">
+      <c r="A344" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="B344" s="9" t="s">
+      <c r="B344" s="66" t="s">
         <v>333</v>
       </c>
-      <c r="C344" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="345" spans="1:3" ht="21">
-      <c r="A345" s="8" t="s">
+      <c r="C344" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" s="47" customFormat="1" ht="21">
+      <c r="A345" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="B345" s="6" t="s">
+      <c r="B345" s="24" t="s">
         <v>334</v>
       </c>
-      <c r="C345" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="346" spans="1:3" ht="21">
-      <c r="A346" s="8" t="s">
+      <c r="C345" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" s="48" customFormat="1" ht="21">
+      <c r="A346" s="32" t="s">
         <v>324</v>
       </c>
-      <c r="B346" s="6" t="s">
+      <c r="B346" s="21" t="s">
         <v>335</v>
       </c>
-      <c r="C346" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="347" spans="1:3" ht="21">
-      <c r="A347" s="8" t="s">
+      <c r="C346" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" s="47" customFormat="1" ht="21">
+      <c r="A347" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="B347" s="6" t="s">
+      <c r="B347" s="24" t="s">
         <v>336</v>
       </c>
-      <c r="C347" s="4" t="s">
+      <c r="C347" s="25" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>